<commit_message>
WIP: Sample 6, draft page
</commit_message>
<xml_diff>
--- a/EPPlus.WebSampleMvc.NetCore/data/SwedishGeography.xlsx
+++ b/EPPlus.WebSampleMvc.NetCore/data/SwedishGeography.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MatsAlm\dev\EPPlusSoftware\EPPlus6.WebSamples\EPPlus.WebSampleMvc.NetCore\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{26970A82-9BFC-4E5F-9BED-D0EA38014CFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAA6BE75-E638-467E-A028-853798ACC3C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" xr2:uid="{C0568D70-DEBA-4913-AD40-3009A6F4C49A}"/>
   </bookViews>
@@ -82,9 +82,6 @@
     <t>Västmanland</t>
   </si>
   <si>
-    <t>Area</t>
-  </si>
-  <si>
     <t>Max depth</t>
   </si>
   <si>
@@ -116,6 +113,9 @@
   </si>
   <si>
     <t>Largest lakes in Sweden</t>
+  </si>
+  <si>
+    <t>Area (km2)</t>
   </si>
 </sst>
 </file>
@@ -146,13 +146,31 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -340,35 +358,41 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -686,7 +710,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -695,22 +719,24 @@
     <col min="2" max="2" width="13.41796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.05078125" customWidth="1"/>
     <col min="4" max="4" width="9.7890625" customWidth="1"/>
-    <col min="10" max="10" width="12.1015625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.68359375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.47265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.62890625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="G1" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="G1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
     </row>
     <row r="2" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="3" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -720,71 +746,71 @@
       <c r="B3" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="21" t="s">
         <v>4</v>
       </c>
       <c r="G3" s="17" t="s">
         <v>1</v>
       </c>
       <c r="H3" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="18" t="s">
+      <c r="J3" s="19" t="s">
         <v>16</v>
-      </c>
-      <c r="J3" s="21" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="8">
         <v>952058</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="9">
         <v>2205105</v>
       </c>
-      <c r="G4" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" s="11">
+      <c r="G4" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="7">
         <v>5650</v>
       </c>
       <c r="I4" s="11">
         <v>106</v>
       </c>
-      <c r="J4" s="16">
+      <c r="J4" s="12">
         <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>565496</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="3">
         <v>1015974</v>
       </c>
-      <c r="G5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="2">
+      <c r="G5" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="1">
         <v>1893</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="13">
         <v>128</v>
       </c>
       <c r="J5" s="14">
@@ -792,25 +818,25 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>334987</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="3">
         <v>689206</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" s="2">
+      <c r="G6" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="1">
         <v>1072</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="13">
         <v>66</v>
       </c>
       <c r="J6" s="14">
@@ -818,25 +844,25 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>221141</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="3">
         <v>257200</v>
       </c>
-      <c r="G7" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H7" s="2">
+      <c r="G7" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="1">
         <v>483</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="13">
         <v>20</v>
       </c>
       <c r="J7" s="14">
@@ -844,25 +870,25 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>158953</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="3">
         <v>189000</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H8" s="2">
+      <c r="G8" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="1">
         <v>456</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="13">
         <v>74</v>
       </c>
       <c r="J8" s="14">
@@ -870,25 +896,25 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>150949</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="3">
         <v>196700</v>
       </c>
-      <c r="G9" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H9" s="2">
+      <c r="G9" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="1">
         <v>330</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="13">
         <v>168</v>
       </c>
       <c r="J9" s="14">
@@ -896,28 +922,28 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="5">
         <v>150564</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="6">
         <v>169200</v>
       </c>
-      <c r="G10" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="H10" s="7">
+      <c r="G10" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="4">
         <v>292</v>
       </c>
-      <c r="I10" s="7">
+      <c r="I10" s="15">
         <v>134</v>
       </c>
-      <c r="J10" s="15">
+      <c r="J10" s="16">
         <v>28</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed typo in SwedishGeography.xlsx
</commit_message>
<xml_diff>
--- a/EPPlus.WebSampleMvc.NetCore/data/SwedishGeography.xlsx
+++ b/EPPlus.WebSampleMvc.NetCore/data/SwedishGeography.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mats\dev\EPPlusSoftware\EPPlus6.WebSamples\EPPlus.WebSampleMvc.NetCore\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C359D4C-0C2A-46D3-94A1-ABA2DFF246E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B082EB24-DD28-4310-82A8-B2A412EB2E26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="95880" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{C0568D70-DEBA-4913-AD40-3009A6F4C49A}"/>
+    <workbookView xWindow="95880" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{C0568D70-DEBA-4913-AD40-3009A6F4C49A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1535,12 +1535,6 @@
     <t>Municipality</t>
   </si>
   <si>
-    <t>Lake1</t>
-  </si>
-  <si>
-    <t>Lake2</t>
-  </si>
-  <si>
     <t>Sea</t>
   </si>
   <si>
@@ -1692,6 +1686,34 @@
       <t>Christine Stigsdatter of Hvide</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t>Lake</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>²</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Lake</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>¹</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -1701,7 +1723,7 @@
     <numFmt numFmtId="164" formatCode="0&quot; m&quot;"/>
     <numFmt numFmtId="165" formatCode="#,##0&quot; km2&quot;"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1776,6 +1798,12 @@
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -2263,96 +2291,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -2366,6 +2304,96 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3104,8 +3132,8 @@
     <tableColumn id="4" xr3:uid="{04E7ED36-AA93-4A6E-B3A2-5818046AE0D9}" name="Population" dataDxfId="4"/>
     <tableColumn id="5" xr3:uid="{D70724C4-45B3-40C4-81DE-85649872752A}" name="Area" dataDxfId="3"/>
     <tableColumn id="6" xr3:uid="{6A61369F-FFA1-4B0D-B47D-C06415860503}" name="Land" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{5409F2D9-6C5B-4FC1-A312-F961DB094CC6}" name="Lake1" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{23E4AE68-197D-48F1-865A-98717395C332}" name="Lake2" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{5409F2D9-6C5B-4FC1-A312-F961DB094CC6}" name="Lake¹" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{23E4AE68-197D-48F1-865A-98717395C332}" name="Lake²" dataDxfId="0"/>
     <tableColumn id="9" xr3:uid="{1A3E57FF-360B-4801-9E67-98028DEB6DF8}" name="Sea"/>
     <tableColumn id="10" xr3:uid="{2972DF5F-6F1F-4F79-8E3D-9F63B74CEB85}" name="Density"/>
   </tableColumns>
@@ -3428,18 +3456,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21" x14ac:dyDescent="1">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="G1" s="62" t="s">
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="G1" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
     </row>
     <row r="2" spans="1:10" ht="15.5" thickBot="1" x14ac:dyDescent="0.9"/>
     <row r="3" spans="1:10" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
@@ -3664,7 +3692,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE48F505-2217-46F4-B0DD-E2FA40115D4B}">
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H57" sqref="H57"/>
     </sheetView>
   </sheetViews>
@@ -3698,14 +3726,14 @@
       <c r="A2" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="83" t="s">
+      <c r="B2" s="71"/>
+      <c r="C2" s="74" t="s">
         <v>31</v>
       </c>
       <c r="D2" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="69" t="s">
+      <c r="E2" s="77" t="s">
         <v>33</v>
       </c>
     </row>
@@ -3713,136 +3741,136 @@
       <c r="A3" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="64"/>
-      <c r="C3" s="84"/>
+      <c r="B3" s="72"/>
+      <c r="C3" s="75"/>
       <c r="D3" s="25"/>
-      <c r="E3" s="70"/>
+      <c r="E3" s="78"/>
     </row>
     <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.75">
       <c r="A4" s="24"/>
-      <c r="B4" s="64"/>
-      <c r="C4" s="84"/>
+      <c r="B4" s="72"/>
+      <c r="C4" s="75"/>
       <c r="D4" s="25"/>
-      <c r="E4" s="70"/>
+      <c r="E4" s="78"/>
     </row>
     <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.75">
       <c r="A5" s="24"/>
-      <c r="B5" s="64"/>
-      <c r="C5" s="84"/>
+      <c r="B5" s="72"/>
+      <c r="C5" s="75"/>
       <c r="D5" s="25"/>
-      <c r="E5" s="70"/>
+      <c r="E5" s="78"/>
     </row>
     <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.75">
       <c r="A6" s="24"/>
-      <c r="B6" s="64"/>
-      <c r="C6" s="84"/>
+      <c r="B6" s="72"/>
+      <c r="C6" s="75"/>
       <c r="D6" s="25"/>
-      <c r="E6" s="70"/>
+      <c r="E6" s="78"/>
     </row>
     <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.75">
       <c r="A7" s="24"/>
-      <c r="B7" s="64"/>
-      <c r="C7" s="84"/>
+      <c r="B7" s="72"/>
+      <c r="C7" s="75"/>
       <c r="D7" s="25"/>
-      <c r="E7" s="70"/>
+      <c r="E7" s="78"/>
     </row>
     <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.75">
       <c r="A8" s="24"/>
-      <c r="B8" s="64"/>
-      <c r="C8" s="84"/>
+      <c r="B8" s="72"/>
+      <c r="C8" s="75"/>
       <c r="D8" s="26"/>
-      <c r="E8" s="70"/>
+      <c r="E8" s="78"/>
     </row>
     <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.75">
       <c r="A9" s="27"/>
-      <c r="B9" s="65"/>
-      <c r="C9" s="85"/>
+      <c r="B9" s="73"/>
+      <c r="C9" s="76"/>
       <c r="D9" s="28"/>
-      <c r="E9" s="71"/>
+      <c r="E9" s="79"/>
     </row>
     <row r="10" spans="1:5" ht="45.75" x14ac:dyDescent="0.75">
-      <c r="A10" s="86" t="s">
+      <c r="A10" s="68" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="63"/>
-      <c r="C10" s="83" t="s">
+      <c r="B10" s="71"/>
+      <c r="C10" s="74" t="s">
         <v>36</v>
       </c>
       <c r="D10" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="69" t="s">
+      <c r="E10" s="77" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.75">
-      <c r="A11" s="87"/>
-      <c r="B11" s="64"/>
-      <c r="C11" s="84"/>
+      <c r="A11" s="69"/>
+      <c r="B11" s="72"/>
+      <c r="C11" s="75"/>
       <c r="D11" s="25"/>
-      <c r="E11" s="70"/>
+      <c r="E11" s="78"/>
     </row>
     <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.75">
-      <c r="A12" s="87"/>
-      <c r="B12" s="64"/>
-      <c r="C12" s="84"/>
+      <c r="A12" s="69"/>
+      <c r="B12" s="72"/>
+      <c r="C12" s="75"/>
       <c r="D12" s="25"/>
-      <c r="E12" s="70"/>
+      <c r="E12" s="78"/>
     </row>
     <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.75">
-      <c r="A13" s="87"/>
-      <c r="B13" s="64"/>
-      <c r="C13" s="84"/>
+      <c r="A13" s="69"/>
+      <c r="B13" s="72"/>
+      <c r="C13" s="75"/>
       <c r="D13" s="25"/>
-      <c r="E13" s="70"/>
+      <c r="E13" s="78"/>
     </row>
     <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.75">
-      <c r="A14" s="87"/>
-      <c r="B14" s="64"/>
-      <c r="C14" s="84"/>
+      <c r="A14" s="69"/>
+      <c r="B14" s="72"/>
+      <c r="C14" s="75"/>
       <c r="D14" s="25"/>
-      <c r="E14" s="70"/>
+      <c r="E14" s="78"/>
     </row>
     <row r="15" spans="1:5" ht="15.25" x14ac:dyDescent="0.75">
-      <c r="A15" s="87"/>
-      <c r="B15" s="64"/>
-      <c r="C15" s="84"/>
+      <c r="A15" s="69"/>
+      <c r="B15" s="72"/>
+      <c r="C15" s="75"/>
       <c r="D15" s="30"/>
-      <c r="E15" s="70"/>
+      <c r="E15" s="78"/>
     </row>
     <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.75">
-      <c r="A16" s="87"/>
-      <c r="B16" s="64"/>
-      <c r="C16" s="84"/>
+      <c r="A16" s="69"/>
+      <c r="B16" s="72"/>
+      <c r="C16" s="75"/>
       <c r="D16" s="31"/>
-      <c r="E16" s="70"/>
+      <c r="E16" s="78"/>
     </row>
     <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.75">
-      <c r="A17" s="87"/>
-      <c r="B17" s="64"/>
-      <c r="C17" s="84"/>
+      <c r="A17" s="69"/>
+      <c r="B17" s="72"/>
+      <c r="C17" s="75"/>
       <c r="D17" s="26"/>
-      <c r="E17" s="70"/>
+      <c r="E17" s="78"/>
     </row>
     <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.75">
-      <c r="A18" s="88"/>
-      <c r="B18" s="65"/>
-      <c r="C18" s="85"/>
+      <c r="A18" s="70"/>
+      <c r="B18" s="73"/>
+      <c r="C18" s="76"/>
       <c r="D18" s="28"/>
-      <c r="E18" s="71"/>
+      <c r="E18" s="79"/>
     </row>
     <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.75">
       <c r="A19" s="32" t="s">
         <v>39</v>
       </c>
       <c r="B19" s="33"/>
-      <c r="C19" s="83" t="s">
+      <c r="C19" s="74" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="89" t="s">
+      <c r="D19" s="83" t="s">
         <v>41</v>
       </c>
-      <c r="E19" s="69" t="s">
+      <c r="E19" s="77" t="s">
         <v>42</v>
       </c>
     </row>
@@ -3851,52 +3879,52 @@
         <v>43</v>
       </c>
       <c r="B20" s="35"/>
-      <c r="C20" s="84"/>
-      <c r="D20" s="90"/>
-      <c r="E20" s="70"/>
+      <c r="C20" s="75"/>
+      <c r="D20" s="84"/>
+      <c r="E20" s="78"/>
     </row>
     <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.75">
       <c r="A21" s="34"/>
       <c r="B21" s="35"/>
-      <c r="C21" s="84"/>
-      <c r="D21" s="90"/>
-      <c r="E21" s="70"/>
+      <c r="C21" s="75"/>
+      <c r="D21" s="84"/>
+      <c r="E21" s="78"/>
     </row>
     <row r="22" spans="1:5" ht="16" x14ac:dyDescent="0.75">
       <c r="A22" s="34"/>
       <c r="B22" s="35"/>
-      <c r="C22" s="84"/>
-      <c r="D22" s="90"/>
-      <c r="E22" s="70"/>
+      <c r="C22" s="75"/>
+      <c r="D22" s="84"/>
+      <c r="E22" s="78"/>
     </row>
     <row r="23" spans="1:5" ht="15.25" x14ac:dyDescent="0.75">
       <c r="A23" s="34"/>
       <c r="B23" s="36"/>
-      <c r="C23" s="84"/>
-      <c r="D23" s="90"/>
-      <c r="E23" s="70"/>
+      <c r="C23" s="75"/>
+      <c r="D23" s="84"/>
+      <c r="E23" s="78"/>
     </row>
     <row r="24" spans="1:5" ht="15.25" x14ac:dyDescent="0.75">
       <c r="A24" s="37"/>
       <c r="B24" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="C24" s="85"/>
-      <c r="D24" s="91"/>
-      <c r="E24" s="71"/>
+      <c r="C24" s="76"/>
+      <c r="D24" s="85"/>
+      <c r="E24" s="79"/>
     </row>
     <row r="25" spans="1:5" ht="16" x14ac:dyDescent="0.75">
       <c r="A25" s="22" t="s">
         <v>45</v>
       </c>
       <c r="B25" s="33"/>
-      <c r="C25" s="83" t="s">
-        <v>404</v>
+      <c r="C25" s="74" t="s">
+        <v>402</v>
       </c>
       <c r="D25" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="E25" s="74" t="s">
+      <c r="E25" s="80" t="s">
         <v>47</v>
       </c>
     </row>
@@ -3905,77 +3933,77 @@
         <v>48</v>
       </c>
       <c r="B26" s="35"/>
-      <c r="C26" s="84"/>
+      <c r="C26" s="75"/>
       <c r="D26" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="E26" s="79"/>
+      <c r="E26" s="81"/>
     </row>
     <row r="27" spans="1:5" ht="16" x14ac:dyDescent="0.75">
       <c r="A27" s="24"/>
       <c r="B27" s="35"/>
-      <c r="C27" s="84"/>
+      <c r="C27" s="75"/>
       <c r="D27" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="E27" s="79"/>
+      <c r="E27" s="81"/>
     </row>
     <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.75">
       <c r="A28" s="24"/>
       <c r="B28" s="35"/>
-      <c r="C28" s="84"/>
+      <c r="C28" s="75"/>
       <c r="D28" s="39"/>
-      <c r="E28" s="79"/>
+      <c r="E28" s="81"/>
     </row>
     <row r="29" spans="1:5" ht="16" x14ac:dyDescent="0.75">
       <c r="A29" s="24"/>
       <c r="B29" s="35"/>
-      <c r="C29" s="84"/>
+      <c r="C29" s="75"/>
       <c r="D29" s="39"/>
-      <c r="E29" s="79"/>
+      <c r="E29" s="81"/>
     </row>
     <row r="30" spans="1:5" ht="16" x14ac:dyDescent="0.75">
       <c r="A30" s="24"/>
       <c r="B30" s="35"/>
-      <c r="C30" s="84"/>
+      <c r="C30" s="75"/>
       <c r="D30" s="39"/>
-      <c r="E30" s="79"/>
+      <c r="E30" s="81"/>
     </row>
     <row r="31" spans="1:5" ht="16" x14ac:dyDescent="0.75">
       <c r="A31" s="24"/>
       <c r="B31" s="35"/>
-      <c r="C31" s="84"/>
+      <c r="C31" s="75"/>
       <c r="D31" s="39"/>
-      <c r="E31" s="79"/>
+      <c r="E31" s="81"/>
     </row>
     <row r="32" spans="1:5" ht="15.25" x14ac:dyDescent="0.75">
       <c r="A32" s="24"/>
       <c r="B32" s="36"/>
-      <c r="C32" s="84"/>
+      <c r="C32" s="75"/>
       <c r="D32" s="39"/>
-      <c r="E32" s="79"/>
+      <c r="E32" s="81"/>
     </row>
     <row r="33" spans="1:5" ht="15.25" x14ac:dyDescent="0.75">
       <c r="A33" s="27"/>
       <c r="B33" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="C33" s="85"/>
+      <c r="C33" s="76"/>
       <c r="D33" s="40"/>
-      <c r="E33" s="75"/>
+      <c r="E33" s="82"/>
     </row>
     <row r="34" spans="1:5" ht="16" x14ac:dyDescent="0.75">
       <c r="A34" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="B34" s="63"/>
-      <c r="C34" s="83" t="s">
-        <v>405</v>
+      <c r="B34" s="71"/>
+      <c r="C34" s="74" t="s">
+        <v>403</v>
       </c>
       <c r="D34" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="E34" s="69" t="s">
+      <c r="E34" s="77" t="s">
         <v>53</v>
       </c>
     </row>
@@ -3983,189 +4011,189 @@
       <c r="A35" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="B35" s="64"/>
-      <c r="C35" s="84"/>
+      <c r="B35" s="72"/>
+      <c r="C35" s="75"/>
       <c r="D35" s="25"/>
-      <c r="E35" s="70"/>
+      <c r="E35" s="78"/>
     </row>
     <row r="36" spans="1:5" ht="16" x14ac:dyDescent="0.75">
       <c r="A36" s="42"/>
-      <c r="B36" s="64"/>
-      <c r="C36" s="84"/>
+      <c r="B36" s="72"/>
+      <c r="C36" s="75"/>
       <c r="D36" s="25"/>
-      <c r="E36" s="70"/>
+      <c r="E36" s="78"/>
     </row>
     <row r="37" spans="1:5" ht="16" x14ac:dyDescent="0.75">
       <c r="A37" s="42"/>
-      <c r="B37" s="64"/>
-      <c r="C37" s="84"/>
+      <c r="B37" s="72"/>
+      <c r="C37" s="75"/>
       <c r="D37" s="25"/>
-      <c r="E37" s="70"/>
+      <c r="E37" s="78"/>
     </row>
     <row r="38" spans="1:5" ht="15.25" x14ac:dyDescent="0.75">
       <c r="A38" s="42"/>
-      <c r="B38" s="64"/>
-      <c r="C38" s="84"/>
+      <c r="B38" s="72"/>
+      <c r="C38" s="75"/>
       <c r="D38" s="39"/>
-      <c r="E38" s="70"/>
+      <c r="E38" s="78"/>
     </row>
     <row r="39" spans="1:5" ht="16" x14ac:dyDescent="0.75">
       <c r="A39" s="43"/>
-      <c r="B39" s="65"/>
-      <c r="C39" s="85"/>
+      <c r="B39" s="73"/>
+      <c r="C39" s="76"/>
       <c r="D39" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="E39" s="71"/>
+      <c r="E39" s="79"/>
     </row>
     <row r="40" spans="1:5" ht="15.25" x14ac:dyDescent="0.75">
-      <c r="A40" s="80" t="s">
+      <c r="A40" s="86" t="s">
         <v>56</v>
       </c>
       <c r="B40" s="33"/>
-      <c r="C40" s="83" t="s">
-        <v>406</v>
-      </c>
-      <c r="D40" s="66" t="s">
+      <c r="C40" s="74" t="s">
+        <v>404</v>
+      </c>
+      <c r="D40" s="89" t="s">
         <v>57</v>
       </c>
-      <c r="E40" s="74" t="s">
+      <c r="E40" s="80" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="16" x14ac:dyDescent="0.75">
-      <c r="A41" s="81"/>
+      <c r="A41" s="87"/>
       <c r="B41" s="35"/>
-      <c r="C41" s="84"/>
-      <c r="D41" s="67"/>
-      <c r="E41" s="79"/>
+      <c r="C41" s="75"/>
+      <c r="D41" s="90"/>
+      <c r="E41" s="81"/>
     </row>
     <row r="42" spans="1:5" ht="16" x14ac:dyDescent="0.75">
-      <c r="A42" s="81"/>
+      <c r="A42" s="87"/>
       <c r="B42" s="35"/>
-      <c r="C42" s="84"/>
-      <c r="D42" s="67"/>
-      <c r="E42" s="79"/>
+      <c r="C42" s="75"/>
+      <c r="D42" s="90"/>
+      <c r="E42" s="81"/>
     </row>
     <row r="43" spans="1:5" ht="16" x14ac:dyDescent="0.75">
-      <c r="A43" s="81"/>
+      <c r="A43" s="87"/>
       <c r="B43" s="35"/>
-      <c r="C43" s="84"/>
-      <c r="D43" s="67"/>
-      <c r="E43" s="79"/>
+      <c r="C43" s="75"/>
+      <c r="D43" s="90"/>
+      <c r="E43" s="81"/>
     </row>
     <row r="44" spans="1:5" ht="16" x14ac:dyDescent="0.75">
-      <c r="A44" s="81"/>
+      <c r="A44" s="87"/>
       <c r="B44" s="35"/>
-      <c r="C44" s="84"/>
-      <c r="D44" s="67"/>
-      <c r="E44" s="79"/>
+      <c r="C44" s="75"/>
+      <c r="D44" s="90"/>
+      <c r="E44" s="81"/>
     </row>
     <row r="45" spans="1:5" ht="16" x14ac:dyDescent="0.75">
-      <c r="A45" s="81"/>
+      <c r="A45" s="87"/>
       <c r="B45" s="35"/>
-      <c r="C45" s="84"/>
-      <c r="D45" s="67"/>
-      <c r="E45" s="79"/>
+      <c r="C45" s="75"/>
+      <c r="D45" s="90"/>
+      <c r="E45" s="81"/>
     </row>
     <row r="46" spans="1:5" ht="15.25" x14ac:dyDescent="0.75">
-      <c r="A46" s="81"/>
+      <c r="A46" s="87"/>
       <c r="B46" s="36"/>
-      <c r="C46" s="84"/>
-      <c r="D46" s="67"/>
-      <c r="E46" s="79"/>
+      <c r="C46" s="75"/>
+      <c r="D46" s="90"/>
+      <c r="E46" s="81"/>
     </row>
     <row r="47" spans="1:5" ht="15.25" x14ac:dyDescent="0.75">
-      <c r="A47" s="82"/>
+      <c r="A47" s="88"/>
       <c r="B47" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="C47" s="85"/>
-      <c r="D47" s="68"/>
-      <c r="E47" s="75"/>
+      <c r="C47" s="76"/>
+      <c r="D47" s="91"/>
+      <c r="E47" s="82"/>
     </row>
     <row r="48" spans="1:5" ht="16" x14ac:dyDescent="0.75">
-      <c r="A48" s="86" t="s">
+      <c r="A48" s="68" t="s">
         <v>59</v>
       </c>
-      <c r="B48" s="63"/>
-      <c r="C48" s="83" t="s">
-        <v>407</v>
+      <c r="B48" s="71"/>
+      <c r="C48" s="74" t="s">
+        <v>405</v>
       </c>
       <c r="D48" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="E48" s="69" t="s">
+      <c r="E48" s="77" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="16" x14ac:dyDescent="0.75">
-      <c r="A49" s="87"/>
-      <c r="B49" s="64"/>
-      <c r="C49" s="84"/>
+      <c r="A49" s="69"/>
+      <c r="B49" s="72"/>
+      <c r="C49" s="75"/>
       <c r="D49" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="E49" s="70"/>
+      <c r="E49" s="78"/>
     </row>
     <row r="50" spans="1:5" ht="16" x14ac:dyDescent="0.75">
-      <c r="A50" s="87"/>
-      <c r="B50" s="64"/>
-      <c r="C50" s="84"/>
+      <c r="A50" s="69"/>
+      <c r="B50" s="72"/>
+      <c r="C50" s="75"/>
       <c r="D50" s="25"/>
-      <c r="E50" s="70"/>
+      <c r="E50" s="78"/>
     </row>
     <row r="51" spans="1:5" ht="16" x14ac:dyDescent="0.75">
-      <c r="A51" s="87"/>
-      <c r="B51" s="64"/>
-      <c r="C51" s="84"/>
+      <c r="A51" s="69"/>
+      <c r="B51" s="72"/>
+      <c r="C51" s="75"/>
       <c r="D51" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="E51" s="70"/>
+      <c r="E51" s="78"/>
     </row>
     <row r="52" spans="1:5" ht="16" x14ac:dyDescent="0.75">
-      <c r="A52" s="87"/>
-      <c r="B52" s="64"/>
-      <c r="C52" s="84"/>
+      <c r="A52" s="69"/>
+      <c r="B52" s="72"/>
+      <c r="C52" s="75"/>
       <c r="D52" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="E52" s="70"/>
+      <c r="E52" s="78"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A53" s="87"/>
-      <c r="B53" s="64"/>
-      <c r="C53" s="84"/>
+      <c r="A53" s="69"/>
+      <c r="B53" s="72"/>
+      <c r="C53" s="75"/>
       <c r="D53" s="46"/>
-      <c r="E53" s="70"/>
+      <c r="E53" s="78"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A54" s="87"/>
-      <c r="B54" s="64"/>
-      <c r="C54" s="84"/>
+      <c r="A54" s="69"/>
+      <c r="B54" s="72"/>
+      <c r="C54" s="75"/>
       <c r="D54" s="46"/>
-      <c r="E54" s="70"/>
+      <c r="E54" s="78"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A55" s="88"/>
-      <c r="B55" s="65"/>
-      <c r="C55" s="85"/>
+      <c r="A55" s="70"/>
+      <c r="B55" s="73"/>
+      <c r="C55" s="76"/>
       <c r="D55" s="46"/>
-      <c r="E55" s="71"/>
+      <c r="E55" s="79"/>
     </row>
     <row r="56" spans="1:5" ht="16" x14ac:dyDescent="0.75">
       <c r="A56" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="B56" s="63"/>
-      <c r="C56" s="66" t="s">
+      <c r="B56" s="71"/>
+      <c r="C56" s="89" t="s">
         <v>65</v>
       </c>
-      <c r="D56" s="76" t="s">
+      <c r="D56" s="92" t="s">
         <v>66</v>
       </c>
-      <c r="E56" s="69" t="s">
+      <c r="E56" s="77" t="s">
         <v>67</v>
       </c>
     </row>
@@ -4173,23 +4201,23 @@
       <c r="A57" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="B57" s="64"/>
-      <c r="C57" s="67"/>
-      <c r="D57" s="77"/>
-      <c r="E57" s="70"/>
+      <c r="B57" s="72"/>
+      <c r="C57" s="90"/>
+      <c r="D57" s="93"/>
+      <c r="E57" s="78"/>
     </row>
     <row r="58" spans="1:5" ht="106.75" x14ac:dyDescent="0.75">
-      <c r="A58" s="92" t="s">
+      <c r="A58" s="62" t="s">
         <v>69</v>
       </c>
-      <c r="B58" s="93"/>
-      <c r="C58" s="94" t="s">
+      <c r="B58" s="63"/>
+      <c r="C58" s="64" t="s">
         <v>70</v>
       </c>
-      <c r="D58" s="95" t="s">
+      <c r="D58" s="65" t="s">
         <v>71</v>
       </c>
-      <c r="E58" s="96" t="s">
+      <c r="E58" s="66" t="s">
         <v>72</v>
       </c>
     </row>
@@ -4197,127 +4225,127 @@
       <c r="A59" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="B59" s="63"/>
-      <c r="C59" s="66" t="s">
+      <c r="B59" s="71"/>
+      <c r="C59" s="89" t="s">
         <v>74</v>
       </c>
-      <c r="D59" s="72" t="s">
+      <c r="D59" s="94" t="s">
         <v>75</v>
       </c>
-      <c r="E59" s="74" t="s">
+      <c r="E59" s="80" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="16" x14ac:dyDescent="0.75">
       <c r="A60" s="48"/>
-      <c r="B60" s="64"/>
-      <c r="C60" s="67"/>
-      <c r="D60" s="78"/>
-      <c r="E60" s="79"/>
+      <c r="B60" s="72"/>
+      <c r="C60" s="90"/>
+      <c r="D60" s="95"/>
+      <c r="E60" s="81"/>
     </row>
     <row r="61" spans="1:5" ht="16" x14ac:dyDescent="0.75">
       <c r="A61" s="48"/>
-      <c r="B61" s="64"/>
-      <c r="C61" s="67"/>
-      <c r="D61" s="78"/>
-      <c r="E61" s="79"/>
+      <c r="B61" s="72"/>
+      <c r="C61" s="90"/>
+      <c r="D61" s="95"/>
+      <c r="E61" s="81"/>
     </row>
     <row r="62" spans="1:5" ht="16" x14ac:dyDescent="0.75">
       <c r="A62" s="48"/>
-      <c r="B62" s="64"/>
-      <c r="C62" s="67"/>
-      <c r="D62" s="78"/>
-      <c r="E62" s="79"/>
+      <c r="B62" s="72"/>
+      <c r="C62" s="90"/>
+      <c r="D62" s="95"/>
+      <c r="E62" s="81"/>
     </row>
     <row r="63" spans="1:5" ht="15.25" x14ac:dyDescent="0.75">
       <c r="A63" s="34"/>
-      <c r="B63" s="64"/>
-      <c r="C63" s="67"/>
-      <c r="D63" s="78"/>
-      <c r="E63" s="79"/>
+      <c r="B63" s="72"/>
+      <c r="C63" s="90"/>
+      <c r="D63" s="95"/>
+      <c r="E63" s="81"/>
     </row>
     <row r="64" spans="1:5" ht="30.5" x14ac:dyDescent="0.75">
       <c r="A64" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="B64" s="65"/>
-      <c r="C64" s="68"/>
-      <c r="D64" s="73"/>
-      <c r="E64" s="75"/>
+      <c r="B64" s="73"/>
+      <c r="C64" s="91"/>
+      <c r="D64" s="96"/>
+      <c r="E64" s="82"/>
     </row>
     <row r="65" spans="1:5" ht="16" x14ac:dyDescent="0.75">
       <c r="A65" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="B65" s="63"/>
-      <c r="C65" s="66" t="s">
+      <c r="B65" s="71"/>
+      <c r="C65" s="89" t="s">
         <v>79</v>
       </c>
       <c r="D65" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="E65" s="69" t="s">
+      <c r="E65" s="77" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="16" x14ac:dyDescent="0.75">
       <c r="A66" s="48"/>
-      <c r="B66" s="64"/>
-      <c r="C66" s="67"/>
+      <c r="B66" s="72"/>
+      <c r="C66" s="90"/>
       <c r="D66" s="25"/>
-      <c r="E66" s="70"/>
+      <c r="E66" s="78"/>
     </row>
     <row r="67" spans="1:5" ht="16" x14ac:dyDescent="0.75">
       <c r="A67" s="48"/>
-      <c r="B67" s="64"/>
-      <c r="C67" s="67"/>
+      <c r="B67" s="72"/>
+      <c r="C67" s="90"/>
       <c r="D67" s="25"/>
-      <c r="E67" s="70"/>
+      <c r="E67" s="78"/>
     </row>
     <row r="68" spans="1:5" ht="16" x14ac:dyDescent="0.75">
       <c r="A68" s="48"/>
-      <c r="B68" s="64"/>
-      <c r="C68" s="67"/>
+      <c r="B68" s="72"/>
+      <c r="C68" s="90"/>
       <c r="D68" s="25"/>
-      <c r="E68" s="70"/>
+      <c r="E68" s="78"/>
     </row>
     <row r="69" spans="1:5" ht="16" x14ac:dyDescent="0.75">
       <c r="A69" s="48"/>
-      <c r="B69" s="64"/>
-      <c r="C69" s="67"/>
+      <c r="B69" s="72"/>
+      <c r="C69" s="90"/>
       <c r="D69" s="30"/>
-      <c r="E69" s="70"/>
+      <c r="E69" s="78"/>
     </row>
     <row r="70" spans="1:5" ht="15.25" x14ac:dyDescent="0.75">
       <c r="A70" s="34"/>
-      <c r="B70" s="64"/>
-      <c r="C70" s="67"/>
+      <c r="B70" s="72"/>
+      <c r="C70" s="90"/>
       <c r="D70" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="E70" s="70"/>
+      <c r="E70" s="78"/>
     </row>
     <row r="71" spans="1:5" ht="30.5" x14ac:dyDescent="0.75">
       <c r="A71" s="37" t="s">
         <v>83</v>
       </c>
-      <c r="B71" s="65"/>
-      <c r="C71" s="68"/>
+      <c r="B71" s="73"/>
+      <c r="C71" s="91"/>
       <c r="D71" s="47"/>
-      <c r="E71" s="71"/>
+      <c r="E71" s="79"/>
     </row>
     <row r="72" spans="1:5" ht="32" x14ac:dyDescent="0.75">
       <c r="A72" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="B72" s="63"/>
-      <c r="C72" s="66" t="s">
+      <c r="B72" s="71"/>
+      <c r="C72" s="89" t="s">
         <v>74</v>
       </c>
-      <c r="D72" s="72" t="s">
+      <c r="D72" s="94" t="s">
         <v>75</v>
       </c>
-      <c r="E72" s="74" t="s">
+      <c r="E72" s="80" t="s">
         <v>76</v>
       </c>
     </row>
@@ -4325,13 +4353,42 @@
       <c r="A73" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="B73" s="65"/>
-      <c r="C73" s="68"/>
-      <c r="D73" s="73"/>
-      <c r="E73" s="75"/>
+      <c r="B73" s="73"/>
+      <c r="C73" s="91"/>
+      <c r="D73" s="96"/>
+      <c r="E73" s="82"/>
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="B65:B71"/>
+    <mergeCell ref="C65:C71"/>
+    <mergeCell ref="E65:E71"/>
+    <mergeCell ref="B72:B73"/>
+    <mergeCell ref="C72:C73"/>
+    <mergeCell ref="D72:D73"/>
+    <mergeCell ref="E72:E73"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="E56:E57"/>
+    <mergeCell ref="B59:B64"/>
+    <mergeCell ref="C59:C64"/>
+    <mergeCell ref="D59:D64"/>
+    <mergeCell ref="E59:E64"/>
+    <mergeCell ref="A40:A47"/>
+    <mergeCell ref="C40:C47"/>
+    <mergeCell ref="D40:D47"/>
+    <mergeCell ref="E40:E47"/>
+    <mergeCell ref="A48:A55"/>
+    <mergeCell ref="B48:B55"/>
+    <mergeCell ref="C48:C55"/>
+    <mergeCell ref="E48:E55"/>
+    <mergeCell ref="B2:B9"/>
+    <mergeCell ref="C2:C9"/>
+    <mergeCell ref="E2:E9"/>
+    <mergeCell ref="C19:C24"/>
+    <mergeCell ref="D19:D24"/>
+    <mergeCell ref="E19:E24"/>
     <mergeCell ref="A10:A18"/>
     <mergeCell ref="B10:B18"/>
     <mergeCell ref="C10:C18"/>
@@ -4341,35 +4398,6 @@
     <mergeCell ref="E34:E39"/>
     <mergeCell ref="C25:C33"/>
     <mergeCell ref="E25:E33"/>
-    <mergeCell ref="B2:B9"/>
-    <mergeCell ref="C2:C9"/>
-    <mergeCell ref="E2:E9"/>
-    <mergeCell ref="C19:C24"/>
-    <mergeCell ref="D19:D24"/>
-    <mergeCell ref="E19:E24"/>
-    <mergeCell ref="A40:A47"/>
-    <mergeCell ref="C40:C47"/>
-    <mergeCell ref="D40:D47"/>
-    <mergeCell ref="E40:E47"/>
-    <mergeCell ref="A48:A55"/>
-    <mergeCell ref="B48:B55"/>
-    <mergeCell ref="C48:C55"/>
-    <mergeCell ref="E48:E55"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="E56:E57"/>
-    <mergeCell ref="B59:B64"/>
-    <mergeCell ref="C59:C64"/>
-    <mergeCell ref="D59:D64"/>
-    <mergeCell ref="E59:E64"/>
-    <mergeCell ref="B65:B71"/>
-    <mergeCell ref="C65:C71"/>
-    <mergeCell ref="E65:E71"/>
-    <mergeCell ref="B72:B73"/>
-    <mergeCell ref="C72:C73"/>
-    <mergeCell ref="D72:D73"/>
-    <mergeCell ref="E72:E73"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" tooltip="Magnus I of Sweden" display="https://en.wikipedia.org/wiki/Magnus_I_of_Sweden" xr:uid="{1B6503C2-77E7-4670-9CDF-8779F4859972}"/>
@@ -4418,8 +4446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8470D1D4-27B5-409A-BF2C-CFE71E360985}">
   <dimension ref="A1:J291"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -4453,16 +4481,16 @@
         <v>86</v>
       </c>
       <c r="G1" s="60" t="s">
+        <v>407</v>
+      </c>
+      <c r="H1" s="60" t="s">
+        <v>406</v>
+      </c>
+      <c r="I1" s="60" t="s">
         <v>400</v>
       </c>
-      <c r="H1" s="60" t="s">
+      <c r="J1" s="60" t="s">
         <v>401</v>
-      </c>
-      <c r="I1" s="60" t="s">
-        <v>402</v>
-      </c>
-      <c r="J1" s="60" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.75">
@@ -13747,8 +13775,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Completed sample 6 and some ui fixes
</commit_message>
<xml_diff>
--- a/EPPlus.WebSampleMvc.NetCore/data/SwedishGeography.xlsx
+++ b/EPPlus.WebSampleMvc.NetCore/data/SwedishGeography.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mats\dev\EPPlusSoftware\EPPlus6.WebSamples\EPPlus.WebSampleMvc.NetCore\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96C4BA6B-0386-4B79-9A3A-22126F9BC898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3AC5A48-221E-4C88-971B-5F7F41E37230}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="96375" yWindow="2235" windowWidth="28800" windowHeight="14940" activeTab="1" xr2:uid="{C0568D70-DEBA-4913-AD40-3009A6F4C49A}"/>
+    <workbookView xWindow="98160" yWindow="2160" windowWidth="28800" windowHeight="14940" activeTab="1" xr2:uid="{C0568D70-DEBA-4913-AD40-3009A6F4C49A}"/>
   </bookViews>
   <sheets>
     <sheet name="Geography" sheetId="1" r:id="rId1"/>
@@ -223,38 +223,6 @@
     <t>1180 son of Canute I Ericson</t>
   </si>
   <si>
-    <r>
-      <t>Died suddenly in fever on Näs Castle, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF0645AD"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Visingsö</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF202122"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>, 10 April 1216, aged about 36, buried at </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF0645AD"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Varnhem Abbey</t>
-    </r>
-  </si>
-  <si>
     <t>31 January 1208 – 10 April 1216</t>
   </si>
   <si>
@@ -265,38 +233,6 @@
   </si>
   <si>
     <t>None</t>
-  </si>
-  <si>
-    <r>
-      <t>Died on </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF0645AD"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Visingsö</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF202122"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>, 10 March 1222, aged about 21, buried at </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF0645AD"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Alvastra Abbey</t>
-    </r>
   </si>
   <si>
     <t>Eric (XI) the Lisp and Lame (Erik läspe och halte),</t>
@@ -1736,6 +1672,70 @@
         <family val="2"/>
       </rPr>
       <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Died suddenly in fever on Näs Castle,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> Visingsö</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF202122"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, 10 April 1216, aged about 36, buried at </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Varnhem Abbey</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Died on </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Visingsö</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF202122"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, 10 March 1222, aged about 21, buried at </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Alvastra Abbey</t>
     </r>
   </si>
 </sst>
@@ -3516,7 +3516,7 @@
         <v>1</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I3" s="11" t="s">
         <v>15</v>
@@ -3721,8 +3721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE48F505-2217-46F4-B0DD-E2FA40115D4B}">
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="H58" sqref="H58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -3757,7 +3757,7 @@
       </c>
       <c r="B2" s="69"/>
       <c r="C2" s="89" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D2" s="23" t="s">
         <v>31</v>
@@ -3829,7 +3829,7 @@
         <v>36</v>
       </c>
       <c r="E10" s="75" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.75">
@@ -3888,7 +3888,7 @@
       <c r="D18" s="28"/>
       <c r="E18" s="77"/>
     </row>
-    <row r="19" spans="1:5" ht="32" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.75">
       <c r="A19" s="32" t="s">
         <v>37</v>
       </c>
@@ -3900,7 +3900,7 @@
         <v>39</v>
       </c>
       <c r="E19" s="75" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.75">
@@ -3948,7 +3948,7 @@
       </c>
       <c r="B25" s="33"/>
       <c r="C25" s="89" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D25" s="23" t="s">
         <v>43</v>
@@ -4027,13 +4027,13 @@
       </c>
       <c r="B34" s="69"/>
       <c r="C34" s="89" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D34" s="23" t="s">
         <v>49</v>
       </c>
       <c r="E34" s="75" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="16" x14ac:dyDescent="0.75">
@@ -4081,7 +4081,7 @@
       </c>
       <c r="B40" s="33"/>
       <c r="C40" s="89" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D40" s="72" t="s">
         <v>53</v>
@@ -4147,13 +4147,13 @@
       </c>
       <c r="B48" s="69"/>
       <c r="C48" s="89" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D48" s="23" t="s">
         <v>56</v>
       </c>
       <c r="E48" s="75" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="16" x14ac:dyDescent="0.75">
@@ -4220,15 +4220,15 @@
         <v>60</v>
       </c>
       <c r="D56" s="82" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="E56" s="75" t="s">
-        <v>61</v>
+        <v>406</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="89" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A57" s="34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B57" s="70"/>
       <c r="C57" s="73"/>
@@ -4237,32 +4237,32 @@
     </row>
     <row r="58" spans="1:5" ht="106.75" x14ac:dyDescent="0.75">
       <c r="A58" s="62" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B58" s="63"/>
       <c r="C58" s="64" t="s">
+        <v>63</v>
+      </c>
+      <c r="D58" s="65" t="s">
         <v>64</v>
       </c>
-      <c r="D58" s="65" t="s">
-        <v>65</v>
-      </c>
       <c r="E58" s="66" t="s">
-        <v>66</v>
+        <v>407</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="32" x14ac:dyDescent="0.75">
       <c r="A59" s="32" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B59" s="69"/>
       <c r="C59" s="72" t="s">
+        <v>66</v>
+      </c>
+      <c r="D59" s="78" t="s">
+        <v>67</v>
+      </c>
+      <c r="E59" s="80" t="s">
         <v>68</v>
-      </c>
-      <c r="D59" s="78" t="s">
-        <v>69</v>
-      </c>
-      <c r="E59" s="80" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="16" x14ac:dyDescent="0.75">
@@ -4295,7 +4295,7 @@
     </row>
     <row r="64" spans="1:5" ht="30.5" x14ac:dyDescent="0.75">
       <c r="A64" s="37" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B64" s="71"/>
       <c r="C64" s="74"/>
@@ -4304,17 +4304,17 @@
     </row>
     <row r="65" spans="1:5" ht="16" x14ac:dyDescent="0.75">
       <c r="A65" s="32" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B65" s="69"/>
       <c r="C65" s="72" t="s">
+        <v>71</v>
+      </c>
+      <c r="D65" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="E65" s="75" t="s">
         <v>73</v>
-      </c>
-      <c r="D65" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="E65" s="75" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="16" x14ac:dyDescent="0.75">
@@ -4350,13 +4350,13 @@
       <c r="B70" s="70"/>
       <c r="C70" s="73"/>
       <c r="D70" s="30" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E70" s="76"/>
     </row>
     <row r="71" spans="1:5" ht="30.5" x14ac:dyDescent="0.75">
       <c r="A71" s="37" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B71" s="71"/>
       <c r="C71" s="74"/>
@@ -4365,22 +4365,22 @@
     </row>
     <row r="72" spans="1:5" ht="32" x14ac:dyDescent="0.75">
       <c r="A72" s="32" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B72" s="69"/>
       <c r="C72" s="72" t="s">
+        <v>66</v>
+      </c>
+      <c r="D72" s="78" t="s">
+        <v>67</v>
+      </c>
+      <c r="E72" s="80" t="s">
         <v>68</v>
-      </c>
-      <c r="D72" s="78" t="s">
-        <v>69</v>
-      </c>
-      <c r="E72" s="80" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="73" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A73" s="37" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B73" s="71"/>
       <c r="C73" s="74"/>
@@ -4477,7 +4477,7 @@
   <dimension ref="A1:J291"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -4494,10 +4494,10 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
@@ -4506,22 +4506,22 @@
         <v>2</v>
       </c>
       <c r="E1" s="60" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F1" s="60" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G1" s="60" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="H1" s="60" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="I1" s="60" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="J1" s="60" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.75">
@@ -4529,10 +4529,10 @@
         <v>1440</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D2" s="58">
         <v>32148</v>
@@ -4561,10 +4561,10 @@
         <v>1489</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D3" s="58">
         <v>41853</v>
@@ -4593,10 +4593,10 @@
         <v>764</v>
       </c>
       <c r="B4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D4" s="58">
         <v>20287</v>
@@ -4625,10 +4625,10 @@
         <v>604</v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D5" s="58">
         <v>6892</v>
@@ -4657,10 +4657,10 @@
         <v>1984</v>
       </c>
       <c r="B6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D6" s="58">
         <v>14100</v>
@@ -4689,10 +4689,10 @@
         <v>2506</v>
       </c>
       <c r="B7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D7" s="58">
         <v>2707</v>
@@ -4721,10 +4721,10 @@
         <v>2505</v>
       </c>
       <c r="B8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D8" s="58">
         <v>6143</v>
@@ -4753,10 +4753,10 @@
         <v>1784</v>
       </c>
       <c r="B9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D9" s="58">
         <v>25854</v>
@@ -4785,10 +4785,10 @@
         <v>1882</v>
       </c>
       <c r="B10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D10" s="58">
         <v>11534</v>
@@ -4817,10 +4817,10 @@
         <v>2084</v>
       </c>
       <c r="B11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D11" s="58">
         <v>22925</v>
@@ -4849,10 +4849,10 @@
         <v>1460</v>
       </c>
       <c r="B12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D12" s="58">
         <v>9409</v>
@@ -4881,10 +4881,10 @@
         <v>2326</v>
       </c>
       <c r="B13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C13" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D13" s="58">
         <v>7135</v>
@@ -4913,10 +4913,10 @@
         <v>2403</v>
       </c>
       <c r="B14" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C14" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D14" s="58">
         <v>2395</v>
@@ -4945,10 +4945,10 @@
         <v>1260</v>
       </c>
       <c r="B15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C15" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D15" s="58">
         <v>15842</v>
@@ -4977,10 +4977,10 @@
         <v>2582</v>
       </c>
       <c r="B16" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D16" s="58">
         <v>28160</v>
@@ -5009,10 +5009,10 @@
         <v>1443</v>
       </c>
       <c r="B17" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C17" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D17" s="58">
         <v>9634</v>
@@ -5041,10 +5041,10 @@
         <v>2183</v>
       </c>
       <c r="B18" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C18" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D18" s="58">
         <v>26753</v>
@@ -5073,10 +5073,10 @@
         <v>885</v>
       </c>
       <c r="B19" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C19" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D19" s="58">
         <v>10895</v>
@@ -5105,10 +5105,10 @@
         <v>2081</v>
       </c>
       <c r="B20" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C20" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D20" s="58">
         <v>52254</v>
@@ -5137,10 +5137,10 @@
         <v>1490</v>
       </c>
       <c r="B21" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D21" s="58">
         <v>114091</v>
@@ -5169,10 +5169,10 @@
         <v>127</v>
       </c>
       <c r="B22" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C22" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D22" s="58">
         <v>95318</v>
@@ -5201,10 +5201,10 @@
         <v>560</v>
       </c>
       <c r="B23" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C23" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D23" s="58">
         <v>5512</v>
@@ -5233,10 +5233,10 @@
         <v>1272</v>
       </c>
       <c r="B24" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C24" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D24" s="58">
         <v>12650</v>
@@ -5265,10 +5265,10 @@
         <v>2305</v>
       </c>
       <c r="B25" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C25" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D25" s="58">
         <v>6175</v>
@@ -5297,10 +5297,10 @@
         <v>1231</v>
       </c>
       <c r="B26" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C26" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D26" s="58">
         <v>19753</v>
@@ -5329,10 +5329,10 @@
         <v>1278</v>
       </c>
       <c r="B27" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C27" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D27" s="58">
         <v>15636</v>
@@ -5361,10 +5361,10 @@
         <v>1438</v>
       </c>
       <c r="B28" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C28" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D28" s="58">
         <v>4756</v>
@@ -5393,10 +5393,10 @@
         <v>162</v>
       </c>
       <c r="B29" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C29" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D29" s="58">
         <v>32803</v>
@@ -5425,10 +5425,10 @@
         <v>1862</v>
       </c>
       <c r="B30" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C30" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D30" s="58">
         <v>9534</v>
@@ -5457,10 +5457,10 @@
         <v>2425</v>
       </c>
       <c r="B31" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C31" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D31" s="58">
         <v>2459</v>
@@ -5489,10 +5489,10 @@
         <v>1730</v>
       </c>
       <c r="B32" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C32" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D32" s="58">
         <v>8490</v>
@@ -5521,10 +5521,10 @@
         <v>125</v>
       </c>
       <c r="B33" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C33" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D33" s="58">
         <v>29096</v>
@@ -5553,10 +5553,10 @@
         <v>686</v>
       </c>
       <c r="B34" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C34" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D34" s="58">
         <v>17834</v>
@@ -5585,10 +5585,10 @@
         <v>862</v>
       </c>
       <c r="B35" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C35" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D35" s="58">
         <v>9329</v>
@@ -5617,10 +5617,10 @@
         <v>381</v>
       </c>
       <c r="B36" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C36" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D36" s="58">
         <v>47489</v>
@@ -5649,10 +5649,10 @@
         <v>484</v>
       </c>
       <c r="B37" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C37" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D37" s="58">
         <v>107593</v>
@@ -5681,10 +5681,10 @@
         <v>1285</v>
       </c>
       <c r="B38" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C38" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D38" s="58">
         <v>34593</v>
@@ -5713,10 +5713,10 @@
         <v>1445</v>
       </c>
       <c r="B39" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C39" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D39" s="58">
         <v>5698</v>
@@ -5745,10 +5745,10 @@
         <v>1982</v>
       </c>
       <c r="B40" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C40" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D40" s="58">
         <v>13319</v>
@@ -5777,10 +5777,10 @@
         <v>1382</v>
       </c>
       <c r="B41" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C41" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D41" s="58">
         <v>46773</v>
@@ -5809,10 +5809,10 @@
         <v>1499</v>
       </c>
       <c r="B42" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C42" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D42" s="58">
         <v>33270</v>
@@ -5841,10 +5841,10 @@
         <v>2080</v>
       </c>
       <c r="B43" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C43" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D43" s="58">
         <v>59837</v>
@@ -5873,10 +5873,10 @@
         <v>1782</v>
       </c>
       <c r="B44" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C44" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D44" s="58">
         <v>10403</v>
@@ -5905,10 +5905,10 @@
         <v>562</v>
       </c>
       <c r="B45" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C45" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D45" s="58">
         <v>21889</v>
@@ -5937,10 +5937,10 @@
         <v>482</v>
       </c>
       <c r="B46" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C46" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D46" s="58">
         <v>16316</v>
@@ -5969,10 +5969,10 @@
         <v>1763</v>
       </c>
       <c r="B47" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C47" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D47" s="58">
         <v>11606</v>
@@ -6001,10 +6001,10 @@
         <v>1439</v>
       </c>
       <c r="B48" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C48" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D48" s="58">
         <v>6576</v>
@@ -6033,10 +6033,10 @@
         <v>2026</v>
       </c>
       <c r="B49" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C49" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D49" s="58">
         <v>10502</v>
@@ -6065,10 +6065,10 @@
         <v>662</v>
       </c>
       <c r="B50" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C50" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D50" s="58">
         <v>29556</v>
@@ -6097,10 +6097,10 @@
         <v>461</v>
       </c>
       <c r="B51" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C51" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D51" s="58">
         <v>11513</v>
@@ -6129,10 +6129,10 @@
         <v>617</v>
       </c>
       <c r="B52" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C52" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D52" s="58">
         <v>9570</v>
@@ -6161,10 +6161,10 @@
         <v>980</v>
       </c>
       <c r="B53" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C53" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D53" s="58">
         <v>61001</v>
@@ -6193,10 +6193,10 @@
         <v>1764</v>
       </c>
       <c r="B54" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C54" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D54" s="58">
         <v>9091</v>
@@ -6225,10 +6225,10 @@
         <v>1444</v>
       </c>
       <c r="B55" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C55" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D55" s="58">
         <v>5730</v>
@@ -6257,10 +6257,10 @@
         <v>1447</v>
       </c>
       <c r="B56" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C56" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D56" s="58">
         <v>5206</v>
@@ -6289,10 +6289,10 @@
         <v>2523</v>
       </c>
       <c r="B57" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C57" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D57" s="58">
         <v>17449</v>
@@ -6321,10 +6321,10 @@
         <v>2180</v>
       </c>
       <c r="B58" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C58" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D58" s="58">
         <v>103136</v>
@@ -6353,10 +6353,10 @@
         <v>1480</v>
       </c>
       <c r="B59" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C59" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D59" s="58">
         <v>587549</v>
@@ -6385,10 +6385,10 @@
         <v>1471</v>
       </c>
       <c r="B60" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C60" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D60" s="58">
         <v>13263</v>
@@ -6417,10 +6417,10 @@
         <v>643</v>
       </c>
       <c r="B61" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C61" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D61" s="58">
         <v>12810</v>
@@ -6449,10 +6449,10 @@
         <v>1783</v>
       </c>
       <c r="B62" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C62" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D62" s="58">
         <v>11553</v>
@@ -6481,10 +6481,10 @@
         <v>1861</v>
       </c>
       <c r="B63" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C63" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D63" s="58">
         <v>16196</v>
@@ -6513,10 +6513,10 @@
         <v>1961</v>
       </c>
       <c r="B64" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C64" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D64" s="58">
         <v>16608</v>
@@ -6545,10 +6545,10 @@
         <v>1380</v>
       </c>
       <c r="B65" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C65" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D65" s="58">
         <v>104573</v>
@@ -6577,10 +6577,10 @@
         <v>1761</v>
       </c>
       <c r="B66" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C66" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D66" s="58">
         <v>16765</v>
@@ -6609,10 +6609,10 @@
         <v>136</v>
       </c>
       <c r="B67" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C67" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D67" s="58">
         <v>95658</v>
@@ -6641,10 +6641,10 @@
         <v>2583</v>
       </c>
       <c r="B68" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C68" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D68" s="58">
         <v>9496</v>
@@ -6673,10 +6673,10 @@
         <v>331</v>
       </c>
       <c r="B69" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C69" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D69" s="58">
         <v>14303</v>
@@ -6705,10 +6705,10 @@
         <v>2083</v>
       </c>
       <c r="B70" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C70" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D70" s="58">
         <v>15458</v>
@@ -6737,10 +6737,10 @@
         <v>1283</v>
       </c>
       <c r="B71" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C71" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D71" s="58">
         <v>150109</v>
@@ -6769,10 +6769,10 @@
         <v>1466</v>
       </c>
       <c r="B72" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C72" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D72" s="58">
         <v>9501</v>
@@ -6801,10 +6801,10 @@
         <v>1497</v>
       </c>
       <c r="B73" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C73" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D73" s="58">
         <v>9233</v>
@@ -6833,10 +6833,10 @@
         <v>2104</v>
       </c>
       <c r="B74" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C74" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D74" s="58">
         <v>9578</v>
@@ -6865,10 +6865,10 @@
         <v>126</v>
       </c>
       <c r="B75" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C75" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D75" s="58">
         <v>113951</v>
@@ -6897,10 +6897,10 @@
         <v>2184</v>
       </c>
       <c r="B76" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C76" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D76" s="58">
         <v>37744</v>
@@ -6929,10 +6929,10 @@
         <v>860</v>
       </c>
       <c r="B77" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C77" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D77" s="58">
         <v>14056</v>
@@ -6961,10 +6961,10 @@
         <v>1315</v>
       </c>
       <c r="B78" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C78" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D78" s="58">
         <v>10619</v>
@@ -6993,10 +6993,10 @@
         <v>305</v>
       </c>
       <c r="B79" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C79" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D79" s="58">
         <v>22344</v>
@@ -7025,10 +7025,10 @@
         <v>1863</v>
       </c>
       <c r="B80" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C80" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D80" s="58">
         <v>6849</v>
@@ -7057,10 +7057,10 @@
         <v>2361</v>
       </c>
       <c r="B81" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C81" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D81" s="58">
         <v>10114</v>
@@ -7089,10 +7089,10 @@
         <v>2280</v>
       </c>
       <c r="B82" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C82" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D82" s="58">
         <v>25012</v>
@@ -7121,10 +7121,10 @@
         <v>1401</v>
       </c>
       <c r="B83" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C83" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D83" s="58">
         <v>39006</v>
@@ -7153,10 +7153,10 @@
         <v>1293</v>
       </c>
       <c r="B84" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C84" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D84" s="58">
         <v>52309</v>
@@ -7185,10 +7185,10 @@
         <v>1284</v>
       </c>
       <c r="B85" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C85" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D85" s="58">
         <v>27589</v>
@@ -7217,10 +7217,10 @@
         <v>821</v>
       </c>
       <c r="B86" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C86" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D86" s="58">
         <v>5645</v>
@@ -7249,10 +7249,10 @@
         <v>1266</v>
       </c>
       <c r="B87" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C87" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D87" s="58">
         <v>15745</v>
@@ -7281,10 +7281,10 @@
         <v>1267</v>
       </c>
       <c r="B88" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C88" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D88" s="58">
         <v>16954</v>
@@ -7313,10 +7313,10 @@
         <v>2510</v>
       </c>
       <c r="B89" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C89" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D89" s="58">
         <v>4780</v>
@@ -7345,10 +7345,10 @@
         <v>123</v>
       </c>
       <c r="B90" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C90" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D90" s="58">
         <v>83170</v>
@@ -7377,10 +7377,10 @@
         <v>680</v>
       </c>
       <c r="B91" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C91" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D91" s="58">
         <v>143579</v>
@@ -7409,10 +7409,10 @@
         <v>2514</v>
       </c>
       <c r="B92" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C92" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D92" s="58">
         <v>15768</v>
@@ -7441,10 +7441,10 @@
         <v>880</v>
       </c>
       <c r="B93" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C93" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D93" s="58">
         <v>71328</v>
@@ -7473,10 +7473,10 @@
         <v>1446</v>
       </c>
       <c r="B94" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C94" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D94" s="58">
         <v>6965</v>
@@ -7505,10 +7505,10 @@
         <v>1082</v>
       </c>
       <c r="B95" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C95" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D95" s="58">
         <v>32226</v>
@@ -7537,10 +7537,10 @@
         <v>1883</v>
       </c>
       <c r="B96" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C96" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D96" s="58">
         <v>30437</v>
@@ -7569,10 +7569,10 @@
         <v>1080</v>
       </c>
       <c r="B97" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C97" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D97" s="58">
         <v>66708</v>
@@ -7601,10 +7601,10 @@
         <v>1780</v>
       </c>
       <c r="B98" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C98" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D98" s="58">
         <v>95408</v>
@@ -7633,10 +7633,10 @@
         <v>483</v>
       </c>
       <c r="B99" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C99" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D99" s="58">
         <v>34764</v>
@@ -7665,10 +7665,10 @@
         <v>1715</v>
       </c>
       <c r="B100" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C100" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D100" s="58">
         <v>12134</v>
@@ -7697,10 +7697,10 @@
         <v>513</v>
       </c>
       <c r="B101" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C101" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D101" s="58">
         <v>10048</v>
@@ -7729,10 +7729,10 @@
         <v>2584</v>
       </c>
       <c r="B102" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C102" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D102" s="58">
         <v>22555</v>
@@ -7761,10 +7761,10 @@
         <v>1276</v>
       </c>
       <c r="B103" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C103" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D103" s="58">
         <v>17783</v>
@@ -7793,10 +7793,10 @@
         <v>330</v>
       </c>
       <c r="B104" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C104" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D104" s="58">
         <v>19818</v>
@@ -7825,10 +7825,10 @@
         <v>2282</v>
       </c>
       <c r="B105" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C105" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D105" s="58">
         <v>18005</v>
@@ -7857,10 +7857,10 @@
         <v>1290</v>
       </c>
       <c r="B106" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C106" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D106" s="58">
         <v>86641</v>
@@ -7889,10 +7889,10 @@
         <v>1781</v>
       </c>
       <c r="B107" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C107" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D107" s="58">
         <v>24099</v>
@@ -7921,10 +7921,10 @@
         <v>2309</v>
       </c>
       <c r="B108" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C108" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D108" s="58">
         <v>15352</v>
@@ -7953,10 +7953,10 @@
         <v>1881</v>
       </c>
       <c r="B109" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C109" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D109" s="58">
         <v>22144</v>
@@ -7985,10 +7985,10 @@
         <v>1384</v>
       </c>
       <c r="B110" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C110" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D110" s="58">
         <v>85301</v>
@@ -8017,10 +8017,10 @@
         <v>1960</v>
       </c>
       <c r="B111" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C111" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D111" s="58">
         <v>8787</v>
@@ -8049,10 +8049,10 @@
         <v>1482</v>
       </c>
       <c r="B112" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C112" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D112" s="58">
         <v>48271</v>
@@ -8081,10 +8081,10 @@
         <v>1261</v>
       </c>
       <c r="B113" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C113" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D113" s="58">
         <v>32341</v>
@@ -8113,10 +8113,10 @@
         <v>1983</v>
       </c>
       <c r="B114" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C114" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D114" s="58">
         <v>26133</v>
@@ -8145,10 +8145,10 @@
         <v>1381</v>
       </c>
       <c r="B115" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C115" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D115" s="58">
         <v>26319</v>
@@ -8177,10 +8177,10 @@
         <v>1282</v>
       </c>
       <c r="B116" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C116" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D116" s="58">
         <v>46488</v>
@@ -8209,10 +8209,10 @@
         <v>1860</v>
       </c>
       <c r="B117" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C117" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D117" s="58">
         <v>5582</v>
@@ -8241,10 +8241,10 @@
         <v>1814</v>
       </c>
       <c r="B118" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C118" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D118" s="58">
         <v>8603</v>
@@ -8273,10 +8273,10 @@
         <v>2029</v>
       </c>
       <c r="B119" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C119" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D119" s="58">
         <v>16012</v>
@@ -8305,10 +8305,10 @@
         <v>1441</v>
       </c>
       <c r="B120" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C120" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D120" s="58">
         <v>43399</v>
@@ -8337,10 +8337,10 @@
         <v>761</v>
       </c>
       <c r="B121" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C121" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D121" s="58">
         <v>8574</v>
@@ -8369,10 +8369,10 @@
         <v>186</v>
       </c>
       <c r="B122" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C122" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D122" s="58">
         <v>48162</v>
@@ -8401,10 +8401,10 @@
         <v>1494</v>
       </c>
       <c r="B123" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C123" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D123" s="58">
         <v>40460</v>
@@ -8433,10 +8433,10 @@
         <v>1462</v>
       </c>
       <c r="B124" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C124" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D124" s="58">
         <v>14509</v>
@@ -8465,10 +8465,10 @@
         <v>1885</v>
       </c>
       <c r="B125" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C125" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D125" s="58">
         <v>23601</v>
@@ -8497,10 +8497,10 @@
         <v>580</v>
       </c>
       <c r="B126" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C126" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D126" s="58">
         <v>165527</v>
@@ -8529,10 +8529,10 @@
         <v>781</v>
       </c>
       <c r="B127" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C127" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D127" s="58">
         <v>28433</v>
@@ -8561,10 +8561,10 @@
         <v>2161</v>
       </c>
       <c r="B128" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C128" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D128" s="58">
         <v>18804</v>
@@ -8593,10 +8593,10 @@
         <v>1864</v>
       </c>
       <c r="B129" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C129" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D129" s="58">
         <v>4604</v>
@@ -8625,10 +8625,10 @@
         <v>1262</v>
       </c>
       <c r="B130" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C130" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D130" s="58">
         <v>24638</v>
@@ -8657,10 +8657,10 @@
         <v>2085</v>
       </c>
       <c r="B131" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C131" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D131" s="58">
         <v>26497</v>
@@ -8689,10 +8689,10 @@
         <v>2580</v>
       </c>
       <c r="B132" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C132" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D132" s="58">
         <v>78867</v>
@@ -8721,10 +8721,10 @@
         <v>1281</v>
       </c>
       <c r="B133" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C133" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D133" s="58">
         <v>127376</v>
@@ -8753,10 +8753,10 @@
         <v>2481</v>
       </c>
       <c r="B134" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C134" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D134" s="58">
         <v>12264</v>
@@ -8785,10 +8785,10 @@
         <v>1484</v>
       </c>
       <c r="B135" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C135" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D135" s="58">
         <v>14266</v>
@@ -8817,10 +8817,10 @@
         <v>1280</v>
       </c>
       <c r="B136" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C136" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D136" s="58">
         <v>351749</v>
@@ -8849,10 +8849,10 @@
         <v>2023</v>
       </c>
       <c r="B137" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C137" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D137" s="58">
         <v>10218</v>
@@ -8881,10 +8881,10 @@
         <v>2418</v>
       </c>
       <c r="B138" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C138" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D138" s="58">
         <v>3034</v>
@@ -8913,10 +8913,10 @@
         <v>1493</v>
       </c>
       <c r="B139" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C139" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D139" s="58">
         <v>24723</v>
@@ -8945,10 +8945,10 @@
         <v>1463</v>
       </c>
       <c r="B140" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C140" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D140" s="58">
         <v>35201</v>
@@ -8977,10 +8977,10 @@
         <v>767</v>
       </c>
       <c r="B141" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C141" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D141" s="58">
         <v>10320</v>
@@ -9009,10 +9009,10 @@
         <v>1461</v>
       </c>
       <c r="B142" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C142" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D142" s="58">
         <v>9268</v>
@@ -9041,10 +9041,10 @@
         <v>586</v>
       </c>
       <c r="B143" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C143" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D143" s="58">
         <v>28269</v>
@@ -9073,10 +9073,10 @@
         <v>2062</v>
       </c>
       <c r="B144" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C144" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D144" s="58">
         <v>20670</v>
@@ -9105,10 +9105,10 @@
         <v>583</v>
       </c>
       <c r="B145" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C145" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D145" s="58">
         <v>43674</v>
@@ -9137,10 +9137,10 @@
         <v>642</v>
       </c>
       <c r="B146" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C146" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D146" s="58">
         <v>7430</v>
@@ -9169,10 +9169,10 @@
         <v>1430</v>
       </c>
       <c r="B147" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C147" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D147" s="58">
         <v>10588</v>
@@ -9201,10 +9201,10 @@
         <v>1762</v>
       </c>
       <c r="B148" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C148" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D148" s="58">
         <v>3680</v>
@@ -9233,10 +9233,10 @@
         <v>1481</v>
       </c>
       <c r="B149" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C149" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D149" s="58">
         <v>69943</v>
@@ -9265,10 +9265,10 @@
         <v>861</v>
       </c>
       <c r="B150" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C150" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D150" s="58">
         <v>13258</v>
@@ -9297,10 +9297,10 @@
         <v>840</v>
       </c>
       <c r="B151" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C151" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D151" s="58">
         <v>15722</v>
@@ -9329,10 +9329,10 @@
         <v>182</v>
       </c>
       <c r="B152" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C152" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D152" s="58">
         <v>108234</v>
@@ -9361,10 +9361,10 @@
         <v>1884</v>
       </c>
       <c r="B153" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C153" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D153" s="58">
         <v>10721</v>
@@ -9393,10 +9393,10 @@
         <v>1962</v>
       </c>
       <c r="B154" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C154" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D154" s="58">
         <v>5714</v>
@@ -9425,10 +9425,10 @@
         <v>2132</v>
       </c>
       <c r="B155" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C155" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D155" s="58">
         <v>9480</v>
@@ -9457,10 +9457,10 @@
         <v>2401</v>
       </c>
       <c r="B156" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C156" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D156" s="58">
         <v>7100</v>
@@ -9489,10 +9489,10 @@
         <v>581</v>
       </c>
       <c r="B157" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C157" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D157" s="58">
         <v>144458</v>
@@ -9521,10 +9521,10 @@
         <v>188</v>
       </c>
       <c r="B158" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C158" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D158" s="58">
         <v>64762</v>
@@ -9553,10 +9553,10 @@
         <v>2417</v>
       </c>
       <c r="B159" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C159" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D159" s="58">
         <v>3971</v>
@@ -9585,10 +9585,10 @@
         <v>881</v>
       </c>
       <c r="B160" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C160" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D160" s="58">
         <v>20284</v>
@@ -9617,10 +9617,10 @@
         <v>140</v>
       </c>
       <c r="B161" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C161" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D161" s="58">
         <v>11500</v>
@@ -9649,10 +9649,10 @@
         <v>480</v>
       </c>
       <c r="B162" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C162" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D162" s="58">
         <v>57633</v>
@@ -9681,10 +9681,10 @@
         <v>192</v>
       </c>
       <c r="B163" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C163" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D163" s="58">
         <v>29495</v>
@@ -9713,10 +9713,10 @@
         <v>682</v>
       </c>
       <c r="B164" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C164" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D164" s="58">
         <v>31782</v>
@@ -9745,10 +9745,10 @@
         <v>2101</v>
       </c>
       <c r="B165" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C165" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D165" s="58">
         <v>5865</v>
@@ -9777,10 +9777,10 @@
         <v>1060</v>
       </c>
       <c r="B166" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C166" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D166" s="58">
         <v>13263</v>
@@ -9809,10 +9809,10 @@
         <v>2034</v>
       </c>
       <c r="B167" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C167" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D167" s="58">
         <v>6918</v>
@@ -9841,10 +9841,10 @@
         <v>1421</v>
       </c>
       <c r="B168" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C168" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D168" s="58">
         <v>15345</v>
@@ -9873,10 +9873,10 @@
         <v>1273</v>
       </c>
       <c r="B169" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C169" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D169" s="58">
         <v>13269</v>
@@ -9905,10 +9905,10 @@
         <v>882</v>
       </c>
       <c r="B170" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C170" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D170" s="58">
         <v>27220</v>
@@ -9937,10 +9937,10 @@
         <v>2121</v>
       </c>
       <c r="B171" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C171" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D171" s="58">
         <v>11711</v>
@@ -9969,10 +9969,10 @@
         <v>481</v>
       </c>
       <c r="B172" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C172" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D172" s="58">
         <v>12132</v>
@@ -10001,10 +10001,10 @@
         <v>2521</v>
       </c>
       <c r="B173" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C173" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D173" s="58">
         <v>5973</v>
@@ -10033,10 +10033,10 @@
         <v>1402</v>
       </c>
       <c r="B174" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C174" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D174" s="58">
         <v>39529</v>
@@ -10065,10 +10065,10 @@
         <v>1275</v>
       </c>
       <c r="B175" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C175" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D175" s="58">
         <v>7565</v>
@@ -10097,10 +10097,10 @@
         <v>2581</v>
       </c>
       <c r="B176" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C176" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D176" s="58">
         <v>42323</v>
@@ -10129,10 +10129,10 @@
         <v>2303</v>
       </c>
       <c r="B177" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C177" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D177" s="58">
         <v>5210</v>
@@ -10161,10 +10161,10 @@
         <v>2409</v>
       </c>
       <c r="B178" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C178" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D178" s="58">
         <v>6786</v>
@@ -10193,10 +10193,10 @@
         <v>1081</v>
       </c>
       <c r="B179" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C179" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D179" s="58">
         <v>29200</v>
@@ -10225,10 +10225,10 @@
         <v>2031</v>
       </c>
       <c r="B180" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C180" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D180" s="58">
         <v>11103</v>
@@ -10257,10 +10257,10 @@
         <v>1981</v>
       </c>
       <c r="B181" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C181" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D181" s="58">
         <v>22998</v>
@@ -10289,10 +10289,10 @@
         <v>128</v>
       </c>
       <c r="B182" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C182" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D182" s="58">
         <v>17252</v>
@@ -10321,10 +10321,10 @@
         <v>2181</v>
       </c>
       <c r="B183" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C183" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D183" s="58">
         <v>39250</v>
@@ -10353,10 +10353,10 @@
         <v>191</v>
       </c>
       <c r="B184" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C184" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D184" s="58">
         <v>50273</v>
@@ -10385,10 +10385,10 @@
         <v>1291</v>
       </c>
       <c r="B185" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C185" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D185" s="58">
         <v>19267</v>
@@ -10417,10 +10417,10 @@
         <v>1265</v>
       </c>
       <c r="B186" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C186" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D186" s="58">
         <v>19497</v>
@@ -10449,10 +10449,10 @@
         <v>1495</v>
       </c>
       <c r="B187" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C187" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D187" s="58">
         <v>18732</v>
@@ -10481,10 +10481,10 @@
         <v>2482</v>
       </c>
       <c r="B188" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C188" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D188" s="58">
         <v>73393</v>
@@ -10513,10 +10513,10 @@
         <v>1904</v>
       </c>
       <c r="B189" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C189" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D189" s="58">
         <v>4371</v>
@@ -10545,10 +10545,10 @@
         <v>1264</v>
       </c>
       <c r="B190" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C190" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D190" s="58">
         <v>16419</v>
@@ -10577,10 +10577,10 @@
         <v>1496</v>
       </c>
       <c r="B191" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C191" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D191" s="58">
         <v>57016</v>
@@ -10609,10 +10609,10 @@
         <v>2061</v>
       </c>
       <c r="B192" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C192" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D192" s="58">
         <v>10933</v>
@@ -10641,10 +10641,10 @@
         <v>2283</v>
       </c>
       <c r="B193" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C193" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D193" s="58">
         <v>18814</v>
@@ -10673,10 +10673,10 @@
         <v>163</v>
       </c>
       <c r="B194" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C194" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D194" s="58">
         <v>75108</v>
@@ -10705,10 +10705,10 @@
         <v>184</v>
       </c>
       <c r="B195" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C195" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D195" s="58">
         <v>84187</v>
@@ -10737,10 +10737,10 @@
         <v>2422</v>
       </c>
       <c r="B196" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C196" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D196" s="58">
         <v>2460</v>
@@ -10769,10 +10769,10 @@
         <v>1427</v>
       </c>
       <c r="B197" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C197" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D197" s="58">
         <v>9125</v>
@@ -10801,10 +10801,10 @@
         <v>1230</v>
       </c>
       <c r="B198" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C198" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D198" s="58">
         <v>26242</v>
@@ -10833,10 +10833,10 @@
         <v>1415</v>
       </c>
       <c r="B199" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C199" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D199" s="58">
         <v>27556</v>
@@ -10865,10 +10865,10 @@
         <v>180</v>
       </c>
       <c r="B200" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C200" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D200" s="58">
         <v>978770</v>
@@ -10897,10 +10897,10 @@
         <v>1760</v>
       </c>
       <c r="B201" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C201" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D201" s="58">
         <v>3948</v>
@@ -10929,10 +10929,10 @@
         <v>2421</v>
       </c>
       <c r="B202" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C202" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D202" s="58">
         <v>5808</v>
@@ -10961,10 +10961,10 @@
         <v>486</v>
       </c>
       <c r="B203" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C203" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D203" s="58">
         <v>38129</v>
@@ -10993,10 +10993,10 @@
         <v>1486</v>
       </c>
       <c r="B204" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C204" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D204" s="58">
         <v>13277</v>
@@ -11025,10 +11025,10 @@
         <v>2313</v>
       </c>
       <c r="B205" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C205" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D205" s="58">
         <v>11473</v>
@@ -11057,10 +11057,10 @@
         <v>183</v>
       </c>
       <c r="B206" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C206" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D206" s="58">
         <v>53564</v>
@@ -11089,10 +11089,10 @@
         <v>2281</v>
       </c>
       <c r="B207" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C207" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D207" s="58">
         <v>99383</v>
@@ -11121,10 +11121,10 @@
         <v>1766</v>
       </c>
       <c r="B208" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C208" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D208" s="58">
         <v>13355</v>
@@ -11153,10 +11153,10 @@
         <v>1907</v>
       </c>
       <c r="B209" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C209" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D209" s="58">
         <v>10099</v>
@@ -11185,10 +11185,10 @@
         <v>1214</v>
       </c>
       <c r="B210" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C210" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D210" s="58">
         <v>14412</v>
@@ -11217,10 +11217,10 @@
         <v>1263</v>
       </c>
       <c r="B211" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C211" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D211" s="58">
         <v>23222</v>
@@ -11249,10 +11249,10 @@
         <v>1465</v>
       </c>
       <c r="B212" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C212" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D212" s="58">
         <v>10864</v>
@@ -11281,10 +11281,10 @@
         <v>1785</v>
       </c>
       <c r="B213" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C213" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D213" s="58">
         <v>15396</v>
@@ -11313,10 +11313,10 @@
         <v>2082</v>
       </c>
       <c r="B214" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C214" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D214" s="58">
         <v>11242</v>
@@ -11345,10 +11345,10 @@
         <v>684</v>
       </c>
       <c r="B215" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C215" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D215" s="58">
         <v>11709</v>
@@ -11377,10 +11377,10 @@
         <v>2182</v>
       </c>
       <c r="B216" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C216" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D216" s="58">
         <v>25446</v>
@@ -11409,10 +11409,10 @@
         <v>582</v>
       </c>
       <c r="B217" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C217" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D217" s="58">
         <v>14673</v>
@@ -11441,10 +11441,10 @@
         <v>181</v>
       </c>
       <c r="B218" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C218" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D218" s="58">
         <v>101209</v>
@@ -11473,10 +11473,10 @@
         <v>1083</v>
       </c>
       <c r="B219" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C219" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D219" s="58">
         <v>17540</v>
@@ -11505,10 +11505,10 @@
         <v>1435</v>
       </c>
       <c r="B220" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C220" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D220" s="58">
         <v>12965</v>
@@ -11537,10 +11537,10 @@
         <v>1472</v>
       </c>
       <c r="B221" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C221" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D221" s="58">
         <v>11281</v>
@@ -11569,10 +11569,10 @@
         <v>1498</v>
       </c>
       <c r="B222" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C222" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D222" s="58">
         <v>12825</v>
@@ -11601,10 +11601,10 @@
         <v>360</v>
       </c>
       <c r="B223" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C223" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D223" s="58">
         <v>21485</v>
@@ -11633,10 +11633,10 @@
         <v>2262</v>
       </c>
       <c r="B224" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C224" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D224" s="58">
         <v>17923</v>
@@ -11665,10 +11665,10 @@
         <v>763</v>
       </c>
       <c r="B225" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C225" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D225" s="58">
         <v>12319</v>
@@ -11697,10 +11697,10 @@
         <v>1419</v>
       </c>
       <c r="B226" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C226" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D226" s="58">
         <v>16312</v>
@@ -11729,10 +11729,10 @@
         <v>1270</v>
       </c>
       <c r="B227" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C227" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D227" s="58">
         <v>13712</v>
@@ -11761,10 +11761,10 @@
         <v>1737</v>
       </c>
       <c r="B228" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C228" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D228" s="58">
         <v>11472</v>
@@ -11793,10 +11793,10 @@
         <v>834</v>
       </c>
       <c r="B229" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C229" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D229" s="58">
         <v>7113</v>
@@ -11825,10 +11825,10 @@
         <v>1452</v>
       </c>
       <c r="B230" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C230" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D230" s="58">
         <v>11937</v>
@@ -11857,10 +11857,10 @@
         <v>687</v>
       </c>
       <c r="B231" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C231" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D231" s="58">
         <v>18874</v>
@@ -11889,10 +11889,10 @@
         <v>1287</v>
       </c>
       <c r="B232" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C232" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D232" s="58">
         <v>46231</v>
@@ -11921,10 +11921,10 @@
         <v>1488</v>
       </c>
       <c r="B233" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C233" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D233" s="58">
         <v>59154</v>
@@ -11953,10 +11953,10 @@
         <v>488</v>
       </c>
       <c r="B234" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C234" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D234" s="58">
         <v>14658</v>
@@ -11985,10 +11985,10 @@
         <v>138</v>
       </c>
       <c r="B235" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C235" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D235" s="58">
         <v>49062</v>
@@ -12017,10 +12017,10 @@
         <v>160</v>
       </c>
       <c r="B236" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C236" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D236" s="58">
         <v>73955</v>
@@ -12049,10 +12049,10 @@
         <v>1473</v>
       </c>
       <c r="B237" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C237" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D237" s="58">
         <v>9207</v>
@@ -12081,10 +12081,10 @@
         <v>1485</v>
       </c>
       <c r="B238" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C238" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D238" s="58">
         <v>57122</v>
@@ -12113,10 +12113,10 @@
         <v>1491</v>
       </c>
       <c r="B239" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C239" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D239" s="58">
         <v>24898</v>
@@ -12145,10 +12145,10 @@
         <v>2480</v>
       </c>
       <c r="B240" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C240" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D240" s="58">
         <v>130997</v>
@@ -12177,10 +12177,10 @@
         <v>114</v>
       </c>
       <c r="B241" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C241" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D241" s="58">
         <v>47820</v>
@@ -12209,10 +12209,10 @@
         <v>139</v>
       </c>
       <c r="B242" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C242" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D242" s="58">
         <v>31082</v>
@@ -12241,10 +12241,10 @@
         <v>380</v>
       </c>
       <c r="B243" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C243" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D243" s="58">
         <v>237596</v>
@@ -12273,10 +12273,10 @@
         <v>760</v>
       </c>
       <c r="B244" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C244" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D244" s="58">
         <v>9449</v>
@@ -12305,10 +12305,10 @@
         <v>584</v>
       </c>
       <c r="B245" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C245" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D245" s="58">
         <v>7528</v>
@@ -12337,10 +12337,10 @@
         <v>665</v>
       </c>
       <c r="B246" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C246" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D246" s="58">
         <v>14746</v>
@@ -12369,10 +12369,10 @@
         <v>563</v>
       </c>
       <c r="B247" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C247" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D247" s="58">
         <v>7660</v>
@@ -12401,10 +12401,10 @@
         <v>115</v>
       </c>
       <c r="B248" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C248" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D248" s="58">
         <v>34246</v>
@@ -12433,10 +12433,10 @@
         <v>2021</v>
       </c>
       <c r="B249" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C249" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D249" s="58">
         <v>6776</v>
@@ -12465,10 +12465,10 @@
         <v>1470</v>
       </c>
       <c r="B250" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C250" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D250" s="58">
         <v>16162</v>
@@ -12497,10 +12497,10 @@
         <v>1383</v>
       </c>
       <c r="B251" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C251" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D251" s="58">
         <v>66658</v>
@@ -12529,10 +12529,10 @@
         <v>187</v>
       </c>
       <c r="B252" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C252" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D252" s="58">
         <v>11996</v>
@@ -12561,10 +12561,10 @@
         <v>1233</v>
       </c>
       <c r="B253" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C253" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D253" s="58">
         <v>37452</v>
@@ -12593,10 +12593,10 @@
         <v>685</v>
       </c>
       <c r="B254" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C254" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D254" s="58">
         <v>27621</v>
@@ -12625,10 +12625,10 @@
         <v>2462</v>
       </c>
       <c r="B255" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C255" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D255" s="58">
         <v>6485</v>
@@ -12657,10 +12657,10 @@
         <v>884</v>
       </c>
       <c r="B256" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C256" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D256" s="58">
         <v>15578</v>
@@ -12689,10 +12689,10 @@
         <v>2404</v>
       </c>
       <c r="B257" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C257" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D257" s="58">
         <v>5550</v>
@@ -12721,10 +12721,10 @@
         <v>428</v>
       </c>
       <c r="B258" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C258" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D258" s="58">
         <v>9063</v>
@@ -12753,10 +12753,10 @@
         <v>1442</v>
       </c>
       <c r="B259" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C259" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D259" s="58">
         <v>12180</v>
@@ -12785,10 +12785,10 @@
         <v>1487</v>
       </c>
       <c r="B260" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C260" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D260" s="58">
         <v>39636</v>
@@ -12817,10 +12817,10 @@
         <v>2460</v>
       </c>
       <c r="B261" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C261" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D261" s="58">
         <v>9054</v>
@@ -12849,10 +12849,10 @@
         <v>120</v>
       </c>
       <c r="B262" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C262" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D262" s="58">
         <v>46232</v>
@@ -12881,10 +12881,10 @@
         <v>683</v>
       </c>
       <c r="B263" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C263" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D263" s="58">
         <v>34661</v>
@@ -12913,10 +12913,10 @@
         <v>883</v>
       </c>
       <c r="B264" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C264" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D264" s="58">
         <v>36747</v>
@@ -12945,10 +12945,10 @@
         <v>1980</v>
       </c>
       <c r="B265" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C265" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D265" s="58">
         <v>156838</v>
@@ -12977,10 +12977,10 @@
         <v>780</v>
       </c>
       <c r="B266" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C266" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D266" s="58">
         <v>95995</v>
@@ -13009,10 +13009,10 @@
         <v>512</v>
       </c>
       <c r="B267" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C267" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D267" s="58">
         <v>3695</v>
@@ -13041,10 +13041,10 @@
         <v>1286</v>
       </c>
       <c r="B268" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C268" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D268" s="58">
         <v>31560</v>
@@ -13073,10 +13073,10 @@
         <v>1492</v>
       </c>
       <c r="B269" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C269" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D269" s="58">
         <v>12318</v>
@@ -13105,10 +13105,10 @@
         <v>2260</v>
       </c>
       <c r="B270" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C270" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D270" s="58">
         <v>9233</v>
@@ -13137,10 +13137,10 @@
         <v>2321</v>
       </c>
       <c r="B271" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C271" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D271" s="58">
         <v>12271</v>
@@ -13169,10 +13169,10 @@
         <v>1765</v>
       </c>
       <c r="B272" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C272" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D272" s="58">
         <v>9942</v>
@@ -13201,10 +13201,10 @@
         <v>2463</v>
       </c>
       <c r="B273" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C273" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D273" s="58">
         <v>2807</v>
@@ -13233,10 +13233,10 @@
         <v>1277</v>
       </c>
       <c r="B274" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C274" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D274" s="58">
         <v>16308</v>
@@ -13265,10 +13265,10 @@
         <v>561</v>
       </c>
       <c r="B275" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C275" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D275" s="58">
         <v>11462</v>
@@ -13297,10 +13297,10 @@
         <v>765</v>
       </c>
       <c r="B276" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C276" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D276" s="58">
         <v>17963</v>
@@ -13329,10 +13329,10 @@
         <v>2039</v>
       </c>
       <c r="B277" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C277" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D277" s="58">
         <v>7042</v>
@@ -13361,10 +13361,10 @@
         <v>319</v>
       </c>
       <c r="B278" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C278" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D278" s="58">
         <v>9627</v>
@@ -13393,10 +13393,10 @@
         <v>2560</v>
       </c>
       <c r="B279" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C279" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D279" s="58">
         <v>8009</v>
@@ -13425,10 +13425,10 @@
         <v>1292</v>
       </c>
       <c r="B280" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C280" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D280" s="58">
         <v>43633</v>
@@ -13457,10 +13457,10 @@
         <v>1407</v>
       </c>
       <c r="B281" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C281" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D281" s="58">
         <v>12902</v>
@@ -13489,10 +13489,10 @@
         <v>509</v>
       </c>
       <c r="B282" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C282" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D282" s="58">
         <v>5309</v>
@@ -13521,10 +13521,10 @@
         <v>1880</v>
       </c>
       <c r="B283" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C283" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D283" s="58">
         <v>156987</v>
@@ -13553,10 +13553,10 @@
         <v>1257</v>
       </c>
       <c r="B284" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C284" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D284" s="58">
         <v>10499</v>
@@ -13585,10 +13585,10 @@
         <v>2284</v>
       </c>
       <c r="B285" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C285" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D285" s="58">
         <v>55823</v>
@@ -13617,10 +13617,10 @@
         <v>2380</v>
       </c>
       <c r="B286" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C286" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D286" s="58">
         <v>64324</v>
@@ -13649,10 +13649,10 @@
         <v>117</v>
       </c>
       <c r="B287" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C287" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D287" s="58">
         <v>48234</v>
@@ -13681,10 +13681,10 @@
         <v>382</v>
       </c>
       <c r="B288" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C288" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D288" s="58">
         <v>22364</v>
@@ -13713,10 +13713,10 @@
         <v>1256</v>
       </c>
       <c r="B289" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C289" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D289" s="58">
         <v>14941</v>
@@ -13745,10 +13745,10 @@
         <v>2513</v>
       </c>
       <c r="B290" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C290" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D290" s="58">
         <v>3252</v>
@@ -13777,10 +13777,10 @@
         <v>2518</v>
       </c>
       <c r="B291" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C291" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D291" s="58">
         <v>4211</v>

</xml_diff>